<commit_message>
Atualização backlog: soma dos pontos de Fibonacci
</commit_message>
<xml_diff>
--- a/documentation/backlog_projIndiv.xlsx
+++ b/documentation/backlog_projIndiv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaura\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaura\OneDrive\Área de Trabalho\1cco_pi_projetoIndividual\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8AC0E0-9F05-4000-8CB3-47150D4647E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043E95DB-DAAA-4928-A47B-B7C2B08E77A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF2AA55B-B245-4FB9-8B2B-69A58253A58D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Permitir a compatibilidade com os navegadores mais conhecidos (Chrome, Edge)</t>
+  </si>
+  <si>
+    <t>Pontos de Fibonacci</t>
   </si>
 </sst>
 </file>
@@ -246,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -254,11 +257,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -267,6 +285,12 @@
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -337,6 +361,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -676,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF66B615-D59F-45A6-AE40-EA7B37B46600}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="63" zoomScaleNormal="45" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="45" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,10 +713,12 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="6" width="25.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="18.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
@@ -696,8 +726,12 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H2"/>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,8 +747,13 @@
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H3"/>
+      <c r="I3" s="5">
+        <f>SUM(F:F)</f>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -731,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -748,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -765,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -782,7 +821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -799,7 +838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -816,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -833,7 +872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
@@ -850,7 +889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
@@ -867,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -884,7 +923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
@@ -901,7 +940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
@@ -918,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>